<commit_message>
adding output excel file and get cdp nei
</commit_message>
<xml_diff>
--- a/spreadsheets/devices.xlsx
+++ b/spreadsheets/devices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cassio/PycharmProjects/get_switches_info/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D22F56A-DA56-344F-B393-55A20DCBA21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1AB453-2371-1A48-BD0A-E0424F986403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14060" yWindow="-28800" windowWidth="68800" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,19 +50,19 @@
     <t>mgmt_ip</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>switch1</t>
   </si>
   <si>
-    <t>1.1.1.1</t>
-  </si>
-  <si>
     <t>switch2</t>
   </si>
   <si>
-    <t>2.2.2.2</t>
+    <t>state</t>
+  </si>
+  <si>
+    <t>192.168.1.101</t>
+  </si>
+  <si>
+    <t>192.168.1.102</t>
   </si>
 </sst>
 </file>
@@ -197,7 +197,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{381CC9EE-E379-3949-8A0B-9662994EC61F}" name="hostname" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{8E625E2F-DFC3-1E47-9623-DFDC9AA7CC26}" name="mgmt_ip" dataDxfId="0"/>
-    <tableColumn id="15" xr3:uid="{4C9C0F45-1D83-3E4C-B741-676088ACCAA4}" name="status"/>
+    <tableColumn id="15" xr3:uid="{4C9C0F45-1D83-3E4C-B741-676088ACCAA4}" name="state"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -503,7 +503,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -520,20 +520,20 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>

</xml_diff>